<commit_message>
+ start on site   + css   + js   + directories (no placeholders yet) + upload mockups
</commit_message>
<xml_diff>
--- a/docs/Log.xlsx
+++ b/docs/Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andrew\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andrew\Dropbox\School\2015\Information Processes &amp; Technology\[AS1] Multimedia Presentation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Create documentation</t>
+  </si>
+  <si>
+    <t>Shaurya</t>
+  </si>
+  <si>
+    <t>Send Project Ara info</t>
   </si>
 </sst>
 </file>
@@ -405,16 +411,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
@@ -432,7 +438,9 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>42037</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -441,6 +449,9 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>42037</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -490,6 +501,17 @@
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>42061</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>